<commit_message>
charts for the user questionnaire
</commit_message>
<xml_diff>
--- a/user-studies/questionnaire.xlsx
+++ b/user-studies/questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/GitHub/master-thesis/user-studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136CBC68-F905-9E43-BC01-F623629F1BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390929C0-F73C-8A40-B549-9CA05F7C4968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="1" xr2:uid="{C4951008-E5A0-7A43-A21A-FC207D5F19CD}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="12">
   <si>
     <t>Chart type</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Which is your</t>
+  </si>
+  <si>
+    <t>Image File</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -885,10 +891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D54A694-7928-1343-8FAA-A407DDF3CB4A}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,7 +905,7 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -915,8 +921,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -932,8 +941,15 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="str">
+        <f>"Q"&amp;IF(LEN(A2)=1,"0","")&amp;A2&amp;".PNG"</f>
+        <v>Q01.PNG</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -949,8 +965,15 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F25" si="0">"Q"&amp;IF(LEN(A3)=1,"0","")&amp;A3&amp;".PNG"</f>
+        <v>Q02.PNG</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -966,8 +989,15 @@
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q03.PNG</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -983,8 +1013,15 @@
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q04.PNG</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1000,8 +1037,15 @@
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q05.PNG</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1017,8 +1061,15 @@
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q06.PNG</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1034,8 +1085,15 @@
       <c r="E8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q07.PNG</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1051,8 +1109,15 @@
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q08.PNG</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1068,8 +1133,15 @@
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q09.PNG</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1085,8 +1157,15 @@
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q10.PNG</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1102,8 +1181,15 @@
       <c r="E12" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q11.PNG</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1119,8 +1205,15 @@
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q12.PNG</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1136,8 +1229,15 @@
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q13.PNG</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1153,8 +1253,15 @@
       <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q14.PNG</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1170,8 +1277,15 @@
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q15.PNG</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1187,8 +1301,15 @@
       <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q16.PNG</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1204,8 +1325,15 @@
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q17.PNG</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1221,8 +1349,15 @@
       <c r="E19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q18.PNG</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1238,8 +1373,15 @@
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q19.PNG</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1255,8 +1397,15 @@
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q20.PNG</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1272,8 +1421,15 @@
       <c r="E22" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q21.PNG</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1289,8 +1445,15 @@
       <c r="E23" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q22.PNG</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1306,8 +1469,15 @@
       <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q23.PNG</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1323,8 +1493,15 @@
       <c r="E25" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q24.PNG</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>

</xml_diff>